<commit_message>
Added chart to report
</commit_message>
<xml_diff>
--- a/doc/results.xlsx
+++ b/doc/results.xlsx
@@ -52,16 +52,16 @@
     <t>d d 3</t>
   </si>
   <si>
-    <t>n w</t>
+    <t>ave. Width without DT</t>
   </si>
   <si>
-    <t>n d</t>
+    <t>ave. Depth without DT</t>
   </si>
   <si>
-    <t>d w</t>
+    <t>ave. Width with DT</t>
   </si>
   <si>
-    <t>d d</t>
+    <t>ave. Depth with DT</t>
   </si>
 </sst>
 </file>
@@ -626,7 +626,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n w</c:v>
+                  <c:v>ave. Width without DT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -806,7 +806,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n d</c:v>
+                  <c:v>ave. Depth without DT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -978,13 +978,16 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>resultnorm1!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ave. Width with DT</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -997,12 +1000,120 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>2.8658535000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0409539999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8658146999999987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7361564999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0833333000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6755726000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4458600000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.8211626666666665</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8233332999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5603341666666668</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9184573</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5822745000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.2241912999999993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.6414425500000007</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7340920000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8809542500000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4076805999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.048217849999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.411429500000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.4398079</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.541847000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.850846499999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.14080665</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.522929100000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.35824465</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.024526649999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.381148</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.63164235</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.099390250000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17.979165999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19.624199000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>18.702477999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19.581780999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.065384000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.895985</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>22.733650000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="4"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
@@ -1010,7 +1121,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>d w</c:v>
+                  <c:v>ave. Depth with DT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1021,141 +1132,6 @@
           <c:val>
             <c:numRef>
               <c:f>resultnorm1!$Q$2:$Q$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="51"/>
-                <c:pt idx="0">
-                  <c:v>2.8658535000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.0409539999999993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.8658146999999987</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.7361564999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0833333000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.6755726000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.4458600000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.8211626666666665</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8233332999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.5603341666666668</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.9184573</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.5822745000000005</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.2241912999999993</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.6414425500000007</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.7340920000000004</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.8809542500000003</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.4076805999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11.048217849999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.411429500000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10.4398079</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11.541847000000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10.850846499999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11.14080665</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>11.522929100000001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>12.35824465</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>11.024526649999999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10.381148</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>10.63164235</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>11.099390250000001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>17.979165999999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>19.624199000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>18.702477999999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>19.581780999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>20.065384000000002</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>20.895985</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>22.733650000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>resultnorm1!$R$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>d d</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>resultnorm1!$R$2:$R$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1326,7 +1302,7 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>295274</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -1636,15 +1612,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:R52"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1687,14 +1663,14 @@
       <c r="O1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
       <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>18.473683999999999</v>
       </c>
@@ -1739,16 +1715,16 @@
         <f>AVERAGE(B2,D2,F2)</f>
         <v>1.5817080599999997</v>
       </c>
-      <c r="Q2">
+      <c r="P2">
         <f>AVERAGE(G2,I2,K2)</f>
         <v>2.8658535000000001</v>
       </c>
-      <c r="R2">
+      <c r="Q2">
         <f>AVERAGE(H2,J2,L2)</f>
         <v>0.92682929999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>17.918800000000001</v>
       </c>
@@ -1793,16 +1769,16 @@
         <f t="shared" ref="O3:O52" si="1">AVERAGE(B3,D3,F3)</f>
         <v>2.8392276666666665</v>
       </c>
+      <c r="P3">
+        <f>AVERAGE(G3,I3,K3)</f>
+        <v>8.0409539999999993</v>
+      </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q52" si="2">AVERAGE(G3,I3,K3)</f>
-        <v>8.0409539999999993</v>
-      </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R37" si="3">AVERAGE(H3,J3,L3)</f>
+        <f t="shared" ref="Q3:Q37" si="2">AVERAGE(H3,J3,L3)</f>
         <v>2.7998812000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>18.555893000000001</v>
       </c>
@@ -1847,16 +1823,16 @@
         <f t="shared" si="1"/>
         <v>2.8461092666666663</v>
       </c>
+      <c r="P4">
+        <f>AVERAGE(G4,I4,K4)</f>
+        <v>6.8658146999999987</v>
+      </c>
       <c r="Q4">
         <f t="shared" si="2"/>
-        <v>6.8658146999999987</v>
-      </c>
-      <c r="R4">
-        <f t="shared" si="3"/>
         <v>0.9361022</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>20.483694</v>
       </c>
@@ -1901,16 +1877,16 @@
         <f t="shared" si="1"/>
         <v>2.8506061999999996</v>
       </c>
+      <c r="P5">
+        <f>AVERAGE(G5,I5,K5)</f>
+        <v>2.7361564999999999</v>
+      </c>
       <c r="Q5">
         <f t="shared" si="2"/>
-        <v>2.7361564999999999</v>
-      </c>
-      <c r="R5">
-        <f t="shared" si="3"/>
         <v>0.94462539999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>19.530343999999999</v>
       </c>
@@ -1955,16 +1931,16 @@
         <f t="shared" si="1"/>
         <v>2.8561109333333334</v>
       </c>
+      <c r="P6">
+        <f>AVERAGE(G6,I6,K6)</f>
+        <v>3.0833333000000001</v>
+      </c>
       <c r="Q6">
         <f t="shared" si="2"/>
-        <v>3.0833333000000001</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="3"/>
         <v>0.94696970000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>19.418976000000001</v>
       </c>
@@ -2009,16 +1985,16 @@
         <f t="shared" si="1"/>
         <v>2.8700987666666666</v>
       </c>
+      <c r="P7">
+        <f>AVERAGE(G7,I7,K7)</f>
+        <v>3.6755726000000002</v>
+      </c>
       <c r="Q7">
         <f t="shared" si="2"/>
-        <v>3.6755726000000002</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="3"/>
         <v>0.94656489999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>20.170687000000001</v>
       </c>
@@ -2063,16 +2039,16 @@
         <f t="shared" si="1"/>
         <v>2.8829101333333331</v>
       </c>
+      <c r="P8">
+        <f>AVERAGE(G8,I8,K8)</f>
+        <v>3.4458600000000001</v>
+      </c>
       <c r="Q8">
         <f t="shared" si="2"/>
-        <v>3.4458600000000001</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="3"/>
         <v>0.94267520000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>20.479279999999999</v>
       </c>
@@ -2117,16 +2093,16 @@
         <f t="shared" si="1"/>
         <v>2.8953639666666668</v>
       </c>
+      <c r="P9">
+        <f>AVERAGE(G9,I9,K9)</f>
+        <v>3.8211626666666665</v>
+      </c>
       <c r="Q9">
         <f t="shared" si="2"/>
-        <v>3.8211626666666665</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="3"/>
         <v>2.2133055533333335</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>18.151378999999999</v>
       </c>
@@ -2171,16 +2147,16 @@
         <f t="shared" si="1"/>
         <v>1.5960256499999999</v>
       </c>
+      <c r="P10">
+        <f>AVERAGE(G10,I10,K10)</f>
+        <v>2.8233332999999998</v>
+      </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>2.8233332999999998</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="3"/>
         <v>0.95333330000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>16.72702</v>
       </c>
@@ -2225,16 +2201,16 @@
         <f t="shared" si="1"/>
         <v>1.5958205666666665</v>
       </c>
+      <c r="P11">
+        <f>AVERAGE(G11,I11,K11)</f>
+        <v>3.5603341666666668</v>
+      </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>3.5603341666666668</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="3"/>
         <v>0.95611386666666665</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>18.470071999999998</v>
       </c>
@@ -2279,16 +2255,16 @@
         <f t="shared" si="1"/>
         <v>2.2341772799999999</v>
       </c>
+      <c r="P12">
+        <f>AVERAGE(G12,I12,K12)</f>
+        <v>3.9184573</v>
+      </c>
       <c r="Q12">
         <f t="shared" si="2"/>
-        <v>3.9184573</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="3"/>
         <v>0.95631363333333341</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>20.465472999999999</v>
       </c>
@@ -2333,16 +2309,16 @@
         <f t="shared" si="1"/>
         <v>2.8859457000000002</v>
       </c>
+      <c r="P13">
+        <f>AVERAGE(G13,I13,K13)</f>
+        <v>5.5822745000000005</v>
+      </c>
       <c r="Q13">
         <f t="shared" si="2"/>
-        <v>5.5822745000000005</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="3"/>
         <v>2.8779649999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>19.021249999999998</v>
       </c>
@@ -2381,16 +2357,16 @@
         <f t="shared" si="1"/>
         <v>1.60645715</v>
       </c>
+      <c r="P14">
+        <f>AVERAGE(G14,I14,K14)</f>
+        <v>5.2241912999999993</v>
+      </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>5.2241912999999993</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="3"/>
         <v>0.96218731999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>21.155752</v>
       </c>
@@ -2429,16 +2405,16 @@
         <f t="shared" si="1"/>
         <v>0.9658346166666667</v>
       </c>
+      <c r="P15">
+        <f>AVERAGE(G15,I15,K15)</f>
+        <v>5.6414425500000007</v>
+      </c>
       <c r="Q15">
         <f t="shared" si="2"/>
-        <v>5.6414425500000007</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="3"/>
         <v>0.96274585000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>19.923649000000001</v>
       </c>
@@ -2477,16 +2453,16 @@
         <f t="shared" si="1"/>
         <v>2.2532918099999999</v>
       </c>
+      <c r="P16">
+        <f>AVERAGE(G16,I16,K16)</f>
+        <v>4.7340920000000004</v>
+      </c>
       <c r="Q16">
         <f t="shared" si="2"/>
-        <v>4.7340920000000004</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="3"/>
         <v>0.96401163000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>18.893003</v>
       </c>
@@ -2525,16 +2501,16 @@
         <f t="shared" si="1"/>
         <v>0.96124134666666672</v>
       </c>
+      <c r="P17">
+        <f>AVERAGE(G17,I17,K17)</f>
+        <v>2.8809542500000003</v>
+      </c>
       <c r="Q17">
         <f t="shared" si="2"/>
-        <v>2.8809542500000003</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="3"/>
         <v>0.96070809999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>19.102419999999999</v>
       </c>
@@ -2573,16 +2549,16 @@
         <f t="shared" si="1"/>
         <v>1.6036274099999999</v>
       </c>
+      <c r="P18">
+        <f>AVERAGE(G18,I18,K18)</f>
+        <v>3.4076805999999999</v>
+      </c>
       <c r="Q18">
         <f t="shared" si="2"/>
-        <v>3.4076805999999999</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="3"/>
         <v>1.8992560749999998</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>20.424147000000001</v>
       </c>
@@ -2621,16 +2597,16 @@
         <f t="shared" si="1"/>
         <v>1.6108968000000001</v>
       </c>
+      <c r="P19">
+        <f>AVERAGE(G19,I19,K19)</f>
+        <v>11.048217849999999</v>
+      </c>
       <c r="Q19">
         <f t="shared" si="2"/>
-        <v>11.048217849999999</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="3"/>
         <v>1.8952219699999999</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>19.225807</v>
       </c>
@@ -2669,16 +2645,16 @@
         <f t="shared" si="1"/>
         <v>1.5880536166666666</v>
       </c>
+      <c r="P20">
+        <f>AVERAGE(G20,I20,K20)</f>
+        <v>10.411429500000001</v>
+      </c>
       <c r="Q20">
         <f t="shared" si="2"/>
-        <v>10.411429500000001</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="3"/>
         <v>1.895172965</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>19.824439999999999</v>
       </c>
@@ -2717,16 +2693,16 @@
         <f t="shared" si="1"/>
         <v>0.96433975999999999</v>
       </c>
+      <c r="P21">
+        <f>AVERAGE(G21,I21,K21)</f>
+        <v>10.4398079</v>
+      </c>
       <c r="Q21">
         <f t="shared" si="2"/>
-        <v>10.4398079</v>
-      </c>
-      <c r="R21">
-        <f t="shared" si="3"/>
         <v>2.8537602999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>19.687822000000001</v>
       </c>
@@ -2765,16 +2741,16 @@
         <f t="shared" si="1"/>
         <v>0.96375185333333346</v>
       </c>
+      <c r="P22">
+        <f>AVERAGE(G22,I22,K22)</f>
+        <v>11.541847000000001</v>
+      </c>
       <c r="Q22">
         <f t="shared" si="2"/>
-        <v>11.541847000000001</v>
-      </c>
-      <c r="R22">
-        <f t="shared" si="3"/>
         <v>1.9043603</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>18.893965000000001</v>
       </c>
@@ -2813,16 +2789,16 @@
         <f t="shared" si="1"/>
         <v>0.96007302333333333</v>
       </c>
+      <c r="P23">
+        <f>AVERAGE(G23,I23,K23)</f>
+        <v>10.850846499999999</v>
+      </c>
       <c r="Q23">
         <f t="shared" si="2"/>
-        <v>10.850846499999999</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="3"/>
         <v>2.87421835</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>18.602616999999999</v>
       </c>
@@ -2861,16 +2837,16 @@
         <f t="shared" si="1"/>
         <v>2.2338765999999999</v>
       </c>
+      <c r="P24">
+        <f>AVERAGE(G24,I24,K24)</f>
+        <v>11.14080665</v>
+      </c>
       <c r="Q24">
         <f t="shared" si="2"/>
-        <v>11.14080665</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="3"/>
         <v>1.91029633</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>17.830819999999999</v>
       </c>
@@ -2909,16 +2885,16 @@
         <f t="shared" si="1"/>
         <v>0.96259736666666662</v>
       </c>
+      <c r="P25">
+        <f>AVERAGE(G25,I25,K25)</f>
+        <v>11.522929100000001</v>
+      </c>
       <c r="Q25">
         <f t="shared" si="2"/>
-        <v>11.522929100000001</v>
-      </c>
-      <c r="R25">
-        <f t="shared" si="3"/>
         <v>2.8844299499999999</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>15.654999999999999</v>
       </c>
@@ -2957,16 +2933,16 @@
         <f t="shared" si="1"/>
         <v>0.96178069999999993</v>
       </c>
+      <c r="P26">
+        <f>AVERAGE(G26,I26,K26)</f>
+        <v>12.35824465</v>
+      </c>
       <c r="Q26">
         <f t="shared" si="2"/>
-        <v>12.35824465</v>
-      </c>
-      <c r="R26">
-        <f t="shared" si="3"/>
         <v>1.9347665699999999</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>17.021715</v>
       </c>
@@ -2999,16 +2975,16 @@
         <f t="shared" si="1"/>
         <v>1.9276740999999999</v>
       </c>
+      <c r="P27">
+        <f>AVERAGE(G27,I27,K27)</f>
+        <v>11.024526649999999</v>
+      </c>
       <c r="Q27">
         <f t="shared" si="2"/>
-        <v>11.024526649999999</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="3"/>
         <v>1.9172174849999999</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>16.476189999999999</v>
       </c>
@@ -3035,16 +3011,16 @@
         <f t="shared" si="1"/>
         <v>0.96687369999999995</v>
       </c>
+      <c r="P28">
+        <f>AVERAGE(G28,I28,K28)</f>
+        <v>10.381148</v>
+      </c>
       <c r="Q28">
         <f t="shared" si="2"/>
-        <v>10.381148</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="3"/>
         <v>2.8920322499999997</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>16.383697999999999</v>
       </c>
@@ -3071,16 +3047,16 @@
         <f t="shared" si="1"/>
         <v>0.97017889999999996</v>
       </c>
+      <c r="P29">
+        <f>AVERAGE(G29,I29,K29)</f>
+        <v>10.63164235</v>
+      </c>
       <c r="Q29">
         <f t="shared" si="2"/>
-        <v>10.63164235</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="3"/>
         <v>1.9207196</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>16.896540000000002</v>
       </c>
@@ -3107,16 +3083,16 @@
         <f t="shared" si="1"/>
         <v>2.9049494</v>
       </c>
+      <c r="P30">
+        <f>AVERAGE(G30,I30,K30)</f>
+        <v>11.099390250000001</v>
+      </c>
       <c r="Q30">
         <f t="shared" si="2"/>
-        <v>11.099390250000001</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="3"/>
         <v>1.9321043499999999</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>17.185873000000001</v>
       </c>
@@ -3137,16 +3113,16 @@
         <f t="shared" si="1"/>
         <v>0.97026020000000002</v>
       </c>
+      <c r="P31">
+        <f>AVERAGE(G31,I31,K31)</f>
+        <v>17.979165999999999</v>
+      </c>
       <c r="Q31">
         <f t="shared" si="2"/>
-        <v>17.979165999999999</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="3"/>
         <v>0.95833330000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>17.377388</v>
       </c>
@@ -3167,16 +3143,16 @@
         <f t="shared" si="1"/>
         <v>2.9290989999999999</v>
       </c>
+      <c r="P32">
+        <f>AVERAGE(G32,I32,K32)</f>
+        <v>19.624199000000001</v>
+      </c>
       <c r="Q32">
         <f t="shared" si="2"/>
-        <v>19.624199000000001</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="3"/>
         <v>2.8750810000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>17.169312000000001</v>
       </c>
@@ -3197,16 +3173,16 @@
         <f t="shared" si="1"/>
         <v>0.97178129999999996</v>
       </c>
+      <c r="P33">
+        <f>AVERAGE(G33,I33,K33)</f>
+        <v>18.702477999999999</v>
+      </c>
       <c r="Q33">
         <f t="shared" si="2"/>
-        <v>18.702477999999999</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="3"/>
         <v>0.9628099</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>16.118556999999999</v>
       </c>
@@ -3227,16 +3203,16 @@
         <f t="shared" si="1"/>
         <v>0.97250859999999995</v>
       </c>
+      <c r="P34">
+        <f>AVERAGE(G34,I34,K34)</f>
+        <v>19.581780999999999</v>
+      </c>
       <c r="Q34">
         <f t="shared" si="2"/>
-        <v>19.581780999999999</v>
-      </c>
-      <c r="R34">
-        <f t="shared" si="3"/>
         <v>0.9627329</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>15.126582000000001</v>
       </c>
@@ -3257,16 +3233,16 @@
         <f t="shared" si="1"/>
         <v>0.97257380000000004</v>
       </c>
+      <c r="P35">
+        <f>AVERAGE(G35,I35,K35)</f>
+        <v>20.065384000000002</v>
+      </c>
       <c r="Q35">
         <f t="shared" si="2"/>
-        <v>20.065384000000002</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="3"/>
         <v>0.96538460000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>17.126064</v>
       </c>
@@ -3287,16 +3263,16 @@
         <f t="shared" si="1"/>
         <v>0.97103919999999999</v>
       </c>
+      <c r="P36">
+        <f>AVERAGE(G36,I36,K36)</f>
+        <v>20.895985</v>
+      </c>
       <c r="Q36">
         <f t="shared" si="2"/>
-        <v>20.895985</v>
-      </c>
-      <c r="R36">
-        <f t="shared" si="3"/>
         <v>0.96532845</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>17.537095999999998</v>
       </c>
@@ -3317,16 +3293,16 @@
         <f t="shared" si="1"/>
         <v>0.97096777000000001</v>
       </c>
+      <c r="P37">
+        <f>AVERAGE(G37,I37,K37)</f>
+        <v>22.733650000000001</v>
+      </c>
       <c r="Q37">
         <f t="shared" si="2"/>
-        <v>22.733650000000001</v>
-      </c>
-      <c r="R37">
-        <f t="shared" si="3"/>
         <v>2.9083111000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>16.953271999999998</v>
       </c>
@@ -3342,7 +3318,7 @@
         <v>0.97009339999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>17.448543999999998</v>
       </c>
@@ -3358,7 +3334,7 @@
         <v>0.96504855</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>14.103536</v>
       </c>
@@ -3374,7 +3350,7 @@
         <v>0.96464645999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>14.012219999999999</v>
       </c>
@@ -3390,7 +3366,7 @@
         <v>2.9255455000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>11.313793</v>
       </c>
@@ -3406,7 +3382,7 @@
         <v>0.96896552999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>13.156342499999999</v>
       </c>
@@ -3422,7 +3398,7 @@
         <v>0.96755164999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>13.555341</v>
       </c>
@@ -3438,7 +3414,7 @@
         <v>2.9255683000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>12.611511</v>
       </c>
@@ -3454,7 +3430,7 @@
         <v>0.97122299999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>13.803167</v>
       </c>
@@ -3470,7 +3446,7 @@
         <v>0.96832580000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>13.515464</v>
       </c>
@@ -3486,7 +3462,7 @@
         <v>0.97319584999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:17">
       <c r="A48">
         <v>13.807205</v>
       </c>

</xml_diff>